<commit_message>
Final steps before delivery
</commit_message>
<xml_diff>
--- a/ergasia3.xlsx
+++ b/ergasia3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\0Uni\Uni\3rd Year\ΠΛΗ24\Εργασία 3\eap-weather\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasga\Desktop\eap2020-24\eap4oetos\pli24\ergasia 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8D3710-7F28-4388-A908-22B167563DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9306B9AF-0C28-4F35-ABA1-27AE5C8ACE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7554518E-40BA-4E82-8E4A-CB1E486DD75E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7554518E-40BA-4E82-8E4A-CB1E486DD75E}"/>
   </bookViews>
   <sheets>
     <sheet name="BS1" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -143,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>Backlog Sprint 1</t>
   </si>
@@ -324,6 +313,15 @@
   </si>
   <si>
     <t>Fetch του weather data και εγγραφή δεδομένων στην βάση</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Διόρθωση και βελτιστοποίηση </t>
+  </si>
+  <si>
+    <t>Εμφάνιση λίστας πόλεων και προβολή ημερομηνιών αναζήτησης</t>
+  </si>
+  <si>
+    <t>Εμφάνιση αριθμού αναζητήσεων και εκτύπωση σε αρχειο .txt</t>
   </si>
 </sst>
 </file>
@@ -711,7 +709,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="el-GR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -838,7 +836,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="184692672"/>
@@ -883,7 +881,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="45454848"/>
@@ -937,7 +935,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="el-GR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -967,7 +965,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="el-GR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1043,7 +1041,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="el-GR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1161,7 +1159,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="184692672"/>
@@ -1206,7 +1204,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="45454848"/>
@@ -1260,7 +1258,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="el-GR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1290,7 +1288,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="el-GR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1366,7 +1364,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="el-GR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1484,7 +1482,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="184692672"/>
@@ -1529,7 +1527,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="el-GR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="45454848"/>
@@ -1583,7 +1581,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="el-GR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1613,7 +1611,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="el-GR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3479,9 +3477,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3519,7 +3517,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3625,7 +3623,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3767,7 +3765,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3778,7 +3776,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3967,7 +3965,9 @@
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
@@ -3985,7 +3985,9 @@
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="D11" s="6" t="s">
         <v>15</v>
       </c>
@@ -4028,7 +4030,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4177,7 +4179,9 @@
       <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="D8" s="6" t="s">
         <v>35</v>
       </c>

</xml_diff>